<commit_message>
neue funktion um einzelnen text anzuzeigen
</commit_message>
<xml_diff>
--- a/testfile.xlsx
+++ b/testfile.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t xml:space="preserve">Frage</t>
   </si>
@@ -40,31 +40,19 @@
     <t xml:space="preserve">Create getter and setter methods for the class.</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/kali/Schreibtisch/cardCreator/setter.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/kali/Schreibtisch/cardCreator/getters.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wie kann man der Klasse den Richtigen sachen geben? Was ist der Unterschied zwischen einem blablabal ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/kali/Schreibtisch/cardCreator/round2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">small</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frage2</t>
+    <t xml:space="preserve">Antwort0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antwort1</t>
   </si>
   <si>
     <t xml:space="preserve">Antwort2</t>
   </si>
   <si>
-    <t xml:space="preserve">Frage3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antwort3</t>
+    <t xml:space="preserve">Wie kann man den Ding am besten machen ?  Wie geht der blabla einfacher?  Was ist die Antwort auf alles?  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
   </si>
   <si>
     <t xml:space="preserve">Frage4</t>
@@ -225,7 +213,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -257,112 +245,108 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
+      <c r="D3" s="2"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
+    <row r="5" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="18.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="3"/>

</xml_diff>

<commit_message>
line break geht voran
</commit_message>
<xml_diff>
--- a/testfile.xlsx
+++ b/testfile.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">s</t>
   </si>
   <si>
-    <t xml:space="preserve">Frage4</t>
+    <t xml:space="preserve">asdfasdfa asdfadsfa asdf asdffad asdfasdfa asdfa afa afaf afa afa afafafa fafaf afsfdasdfasdfa afafasdfadf faas fasdfa</t>
   </si>
   <si>
     <t xml:space="preserve">Antwort4</t>
@@ -213,7 +213,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>